<commit_message>
what is computer science? complete
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\LeeHoang\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\year3\IN3007-IndividualProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EC3886-F209-41FD-AF4B-BEB25C1BE9E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9501A6F7-700B-47C5-984A-AC8DE33217B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
+    <workbookView xWindow="1575" yWindow="2715" windowWidth="27225" windowHeight="11385" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>SZELISKI, R., 2020. COMPUTER VISION. [Place of publication not identified]: SPRINGER NATURE, p.5.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>reference</t>
   </si>
@@ -64,6 +61,25 @@
   </si>
   <si>
     <t>(SZELISKI, 2020)</t>
+  </si>
+  <si>
+    <t>Coifman, B., Beymer, D., McLauchlan, P., &amp; Malik, J. (1998). A real-time computer vision system for vehicle tracking and traffic surveillance. Transportation Research Part C: Emerging Technologies</t>
+  </si>
+  <si>
+    <t>(Coifman, 1998)</t>
+  </si>
+  <si>
+    <t>SZELISKI, R., 2020. COMPUTER VISION. SPRINGER NATURE, p.5.</t>
+  </si>
+  <si>
+    <t>(Hochreiter and
+Schmidhuber, 1997)</t>
+  </si>
+  <si>
+    <t>Deep learning</t>
+  </si>
+  <si>
+    <t>Hochreiter, Sepp and Jurgen Schmidhuber. 1997. "Long Short-Term Memory. Neural Computation" :1735–1780.</t>
   </si>
 </sst>
 </file>
@@ -99,8 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C281B7-8BDC-4908-A351-99DAA93660BA}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -431,44 +450,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>